<commit_message>
Adicionando as funcionalidades de preenchimento das informações para o envio dos contratos e armazenamento de dados de envio
</commit_message>
<xml_diff>
--- a/data/docusign_data.xlsx
+++ b/data/docusign_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DESOUR10\Desktop\Clone das Demandas\admissao\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC97154-DA67-4AA2-97B0-E333913B822E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9C276A-3A6A-4621-A038-A73BA15F8950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1950" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,9 +47,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -79,15 +76,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,102 +383,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4" s="3"/>
-      <c r="F4"/>
-      <c r="G4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5" s="3"/>
-      <c r="F5"/>
-      <c r="G5"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6" s="3"/>
-      <c r="F6"/>
-      <c r="G6"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7" s="3"/>
-      <c r="F7"/>
-      <c r="G7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Definindo as funções de coleta dos contratos a partir dos dados salvos na planilha
</commit_message>
<xml_diff>
--- a/data/docusign_data.xlsx
+++ b/data/docusign_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DESOUR10\Desktop\Clone das Demandas\admissao\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9C276A-3A6A-4621-A038-A73BA15F8950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F2F93A-1844-4315-B87C-93EED33B961C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1950" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -76,10 +76,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -386,19 +389,20 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -414,17 +418,18 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removendo o load_env das dependêcias e corrigindo o caminho do import docusign]
</commit_message>
<xml_diff>
--- a/data/docusign_data.xlsx
+++ b/data/docusign_data.xlsx
@@ -1,64 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DESOUR10\Desktop\Clone das Demandas\admissao\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F2F93A-1844-4315-B87C-93EED33B961C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>RE</t>
-  </si>
-  <si>
-    <t>NOME COMPLETO</t>
-  </si>
-  <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
-    <t>ENVIADO</t>
-  </si>
-  <si>
-    <t>DATA DE ENVIO</t>
-  </si>
-  <si>
-    <t>COLETADO</t>
-  </si>
-  <si>
-    <t>DATA DE COLETA</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -77,27 +46,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -385,51 +413,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col width="9" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="36.7109375" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
+    <col width="27.85546875" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
+    <col width="9.28515625" bestFit="1" customWidth="1" style="1" min="4" max="4"/>
+    <col width="14.85546875" bestFit="1" customWidth="1" style="2" min="5" max="5"/>
+    <col width="10.42578125" bestFit="1" customWidth="1" style="1" min="6" max="6"/>
+    <col width="15.85546875" bestFit="1" customWidth="1" style="2" min="7" max="7"/>
+    <col width="9.140625" customWidth="1" style="1" min="8" max="9"/>
+    <col width="9.140625" customWidth="1" style="1" min="10" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>RE</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>NOME COMPLETO</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>EMAIL</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ENVIADO</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>DATA DE ENVIO</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>COLETADO</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>DATA DE COLETA</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>